<commit_message>
Bunch of minor fixes: * Again, better detection for flipped coords * Luminance calculation to determine if brick should have white or grey details. * More documentation
</commit_message>
<xml_diff>
--- a/Colors/Colors_Master.xlsx
+++ b/Colors/Colors_Master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\brickr\brickr\Colors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usRyaTim\Onedrive - LEGO\Documents\brickr\Colors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECD4211-67B7-488D-B3AD-E057FA58E385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{7ECD4211-67B7-488D-B3AD-E057FA58E385}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{D18FC5E9-F768-4236-ADA1-E219070EED5A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" xr2:uid="{A30B29F7-B580-406F-8677-17DD8856CE58}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A30B29F7-B580-406F-8677-17DD8856CE58}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -159,30 +159,12 @@
     <t>Tr. Brown</t>
   </si>
   <si>
-    <t>Dark Azur</t>
-  </si>
-  <si>
-    <t>Medium Azur</t>
-  </si>
-  <si>
-    <t>Spring Yellowish Green</t>
-  </si>
-  <si>
     <t>Aqua</t>
   </si>
   <si>
-    <t>Olive Green</t>
-  </si>
-  <si>
-    <t>Medium Nougat</t>
-  </si>
-  <si>
     <t>Dark brown</t>
   </si>
   <si>
-    <t>Light Nougat</t>
-  </si>
-  <si>
     <t>White Glow</t>
   </si>
   <si>
@@ -231,13 +213,31 @@
     <t>Vibrant coral</t>
   </si>
   <si>
-    <t>Med. Lavender</t>
-  </si>
-  <si>
     <t>Lavender</t>
   </si>
   <si>
     <t>Palette</t>
+  </si>
+  <si>
+    <t>Olive green</t>
+  </si>
+  <si>
+    <t>Spring yellowish green</t>
+  </si>
+  <si>
+    <t>Medium lavender</t>
+  </si>
+  <si>
+    <t>Medium azur</t>
+  </si>
+  <si>
+    <t>Dark azur</t>
+  </si>
+  <si>
+    <t>Medium nougat</t>
+  </si>
+  <si>
+    <t>Light nougat</t>
   </si>
 </sst>
 </file>
@@ -979,25 +979,25 @@
   <dimension ref="A1:K58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="4.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="4.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" customWidth="1"/>
-    <col min="8" max="9" width="13.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.7265625" style="1"/>
+    <col min="8" max="9" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="42" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="42" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
@@ -1017,22 +1017,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="41" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="H1" s="42" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J1" s="42" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="K1" s="42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>244</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H2" s="1" t="b">
         <v>1</v>
@@ -1065,7 +1065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>5</v>
       </c>
@@ -1083,7 +1083,7 @@
         <v>141</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H3" s="1" t="b">
         <v>1</v>
@@ -1098,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>18</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>90</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H4" s="1" t="b">
         <v>1</v>
@@ -1131,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>21</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H5" s="1" t="b">
         <v>1</v>
@@ -1164,7 +1164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>23</v>
       </c>
@@ -1182,7 +1182,7 @@
         <v>168</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H6" s="1" t="b">
         <v>1</v>
@@ -1197,7 +1197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>24</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>10</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H7" s="1" t="b">
         <v>1</v>
@@ -1230,7 +1230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>26</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>52</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H8" s="1" t="b">
         <v>1</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>28</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>43</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H9" s="1" t="b">
         <v>1</v>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>37</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>65</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H10" s="1" t="b">
         <v>1</v>
@@ -1329,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>38</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>28</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H11" s="1" t="b">
         <v>1</v>
@@ -1362,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>40</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>238</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H12" s="1" t="b">
         <v>1</v>
@@ -1395,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>41</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H13" s="1" t="b">
         <v>1</v>
@@ -1428,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>42</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>237</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H14" s="1" t="b">
         <v>1</v>
@@ -1461,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>184</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H15" s="1" t="b">
         <v>1</v>
@@ -1494,7 +1494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>34</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H16" s="1" t="b">
         <v>1</v>
@@ -1527,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>47</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>41</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H17" s="1" t="b">
         <v>1</v>
@@ -1560,7 +1560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>48</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>100</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H18" s="1" t="b">
         <v>1</v>
@@ -1593,7 +1593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>49</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>91</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H19" s="1" t="b">
         <v>1</v>
@@ -1626,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>102</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>200</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H20" s="1" t="b">
         <v>1</v>
@@ -1659,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>106</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>35</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H21" s="1" t="b">
         <v>1</v>
@@ -1692,7 +1692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>107</v>
       </c>
@@ -1710,7 +1710,7 @@
         <v>148</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H22" s="1" t="b">
         <v>1</v>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>111</v>
       </c>
@@ -1743,7 +1743,7 @@
         <v>158</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H23" s="1" t="b">
         <v>1</v>
@@ -1758,12 +1758,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>113</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="2">
@@ -1776,7 +1776,7 @@
         <v>207</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H24" s="1" t="b">
         <v>1</v>
@@ -1791,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>119</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>24</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H25" s="1" t="b">
         <v>1</v>
@@ -1824,7 +1824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>124</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>118</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H26" s="1" t="b">
         <v>1</v>
@@ -1857,12 +1857,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>126</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C27" s="40"/>
       <c r="D27" s="2">
@@ -1875,7 +1875,7 @@
         <v>184</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H27" s="1" t="b">
         <v>1</v>
@@ -1890,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>135</v>
       </c>
@@ -1908,7 +1908,7 @@
         <v>154</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H28" s="1" t="b">
         <v>1</v>
@@ -1923,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>138</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>98</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H29" s="1" t="b">
         <v>1</v>
@@ -1956,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>140</v>
       </c>
@@ -1974,7 +1974,7 @@
         <v>90</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H30" s="1" t="b">
         <v>1</v>
@@ -1989,7 +1989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>141</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>26</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H31" s="1" t="b">
         <v>1</v>
@@ -2022,7 +2022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>151</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>124</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H32" s="1" t="b">
         <v>1</v>
@@ -2055,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>154</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>18</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H33" s="1" t="b">
         <v>1</v>
@@ -2088,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>191</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H34" s="1" t="b">
         <v>1</v>
@@ -2121,7 +2121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>192</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H35" s="1" t="b">
         <v>1</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>194</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>150</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H36" s="1" t="b">
         <v>1</v>
@@ -2187,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>199</v>
       </c>
@@ -2205,7 +2205,7 @@
         <v>100</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="H37" s="1" t="b">
         <v>1</v>
@@ -2220,12 +2220,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>212</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2">
@@ -2238,7 +2238,7 @@
         <v>247</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H38" s="1" t="b">
         <v>1</v>
@@ -2253,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>221</v>
       </c>
@@ -2271,7 +2271,7 @@
         <v>155</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H39" s="1" t="b">
         <v>1</v>
@@ -2286,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>222</v>
       </c>
@@ -2304,7 +2304,7 @@
         <v>205</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H40" s="1" t="b">
         <v>1</v>
@@ -2319,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>226</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>108</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H41" s="1" t="b">
         <v>1</v>
@@ -2352,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>268</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>145</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H42" s="1" t="b">
         <v>1</v>
@@ -2385,12 +2385,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>283</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
@@ -2403,7 +2403,7 @@
         <v>161</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H43" s="1" t="b">
         <v>1</v>
@@ -2418,12 +2418,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>297</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" s="2">
@@ -2436,7 +2436,7 @@
         <v>34</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H44" s="1" t="b">
         <v>1</v>
@@ -2451,12 +2451,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>308</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" s="2">
@@ -2469,7 +2469,7 @@
         <v>0</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H45" s="1" t="b">
         <v>1</v>
@@ -2484,12 +2484,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>311</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D46" s="1">
         <v>175</v>
@@ -2501,7 +2501,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H46" s="1" t="b">
         <v>1</v>
@@ -2516,12 +2516,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>312</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2">
@@ -2534,7 +2534,7 @@
         <v>85</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H47" s="1" t="b">
         <v>1</v>
@@ -2549,12 +2549,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>315</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2">
@@ -2567,7 +2567,7 @@
         <v>140</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H48" s="1" t="b">
         <v>1</v>
@@ -2582,12 +2582,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>316</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2">
@@ -2600,7 +2600,7 @@
         <v>68</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H49" s="1" t="b">
         <v>1</v>
@@ -2615,12 +2615,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>321</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2">
@@ -2633,7 +2633,7 @@
         <v>195</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H50" s="1" t="b">
         <v>1</v>
@@ -2648,12 +2648,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>322</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
@@ -2666,7 +2666,7 @@
         <v>226</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H51" s="1" t="b">
         <v>1</v>
@@ -2681,12 +2681,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>323</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2">
@@ -2699,7 +2699,7 @@
         <v>234</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H52" s="1" t="b">
         <v>1</v>
@@ -2714,12 +2714,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>324</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2">
@@ -2732,7 +2732,7 @@
         <v>174</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="H53" s="1" t="b">
         <v>1</v>
@@ -2747,12 +2747,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>325</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2">
@@ -2765,7 +2765,7 @@
         <v>222</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H54" s="1" t="b">
         <v>1</v>
@@ -2780,12 +2780,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>326</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2">
@@ -2798,7 +2798,7 @@
         <v>154</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H55" s="1" t="b">
         <v>1</v>
@@ -2813,12 +2813,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>329</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2">
@@ -2831,7 +2831,7 @@
         <v>214</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H56" s="1" t="b">
         <v>1</v>
@@ -2846,12 +2846,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>330</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2">
@@ -2864,7 +2864,7 @@
         <v>79</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H57" s="1" t="b">
         <v>1</v>
@@ -2879,12 +2879,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>353</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C58" s="44"/>
       <c r="D58" s="1">
@@ -2897,7 +2897,7 @@
         <v>120</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="H58" s="1" t="b">
         <v>1</v>

</xml_diff>